<commit_message>
Added BigInt TSB and finished proxies table
</commit_message>
<xml_diff>
--- a/www/evaluation/all_but_onbra.xlsx
+++ b/www/evaluation/all_but_onbra.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/piluc/git/TSBProxy/www/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{2FE53A05-4636-AC45-AFFB-7838BDE35701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{772C727B-9A70-724D-8330-0BA284EC5894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="500" windowWidth="45280" windowHeight="28300" xr2:uid="{B6166BBC-CFA3-9746-8059-366614E28908}"/>
   </bookViews>
@@ -26,16 +26,18 @@
     <definedName name="_02_college_msg_onbra" localSheetId="1">ONBRA!$B$4:$AA$4</definedName>
     <definedName name="_03_email_eu_not_onbra" localSheetId="0">PROXIES!$B$5:$S$5</definedName>
     <definedName name="_03_email_eu_onbra" localSheetId="1">ONBRA!$B$5:$AA$5</definedName>
-    <definedName name="_06_infectious_not_onbra" localSheetId="0">PROXIES!$B$6:$S$6</definedName>
+    <definedName name="_04_bordeaux_not_onbra" localSheetId="0">PROXIES!$B$6:$S$6</definedName>
+    <definedName name="_06_infectious_not_onbra" localSheetId="0">PROXIES!$B$7:$S$7</definedName>
     <definedName name="_06_infectious_onbra" localSheetId="1">ONBRA!$B$6:$AA$6</definedName>
-    <definedName name="_07_SMS_not_onbra" localSheetId="0">PROXIES!$B$7:$S$7</definedName>
+    <definedName name="_07_SMS_not_onbra" localSheetId="0">PROXIES!$B$8:$S$8</definedName>
     <definedName name="_07_SMS_onbra" localSheetId="1">ONBRA!$B$7:$AA$7</definedName>
-    <definedName name="_08_topology_not_onbra" localSheetId="0">PROXIES!$B$8:$S$8</definedName>
-    <definedName name="_09_wiki_elections_not_onbra" localSheetId="0">PROXIES!$B$9:$S$9</definedName>
+    <definedName name="_08_topology_not_onbra" localSheetId="0">PROXIES!$B$9:$S$9</definedName>
+    <definedName name="_09_wiki_elections_not_onbra" localSheetId="0">PROXIES!$B$10:$S$10</definedName>
     <definedName name="_09_wiki_elections_onbra" localSheetId="0">PROXIES!#REF!</definedName>
     <definedName name="_09_wiki_elections_onbra_3" localSheetId="1">ONBRA!$B$9:$AA$9</definedName>
-    <definedName name="_10_facebook_wall_not_onbra" localSheetId="0">PROXIES!$B$10:$S$10</definedName>
-    <definedName name="_11_digg_reply_not_onbra" localSheetId="0">PROXIES!$B$11:$S$11</definedName>
+    <definedName name="_10_facebook_wall_not_onbra" localSheetId="0">PROXIES!$B$11:$S$11</definedName>
+    <definedName name="_10_facebook_wall_onbra" localSheetId="1">ONBRA!$B$10:$AA$10</definedName>
+    <definedName name="_11_digg_reply_not_onbra" localSheetId="0">PROXIES!$B$12:$S$12</definedName>
     <definedName name="_11_digg_reply_onbra" localSheetId="1">ONBRA!#REF!</definedName>
     <definedName name="_11_digg_reply_onbra_3" localSheetId="1">ONBRA!$B$11:$AA$11</definedName>
     <definedName name="_12_mathoverflow_not_onbra" localSheetId="0">PROXIES!#REF!</definedName>
@@ -282,8 +284,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" xr16:uid="{CC6051B5-EC47-9244-A2F6-DFC847CF7A49}" name="06_infectious_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/06_infectious_not_onbra.txt" thousands=" " delimiter=":">
+  <connection id="9" xr16:uid="{4221F4BE-101A-6249-9CED-0FFD2044CFDA}" name="04_bordeaux_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/04_bordeaux_not_onbra.txt" thousands="_x0000_" delimiter=":">
       <textFields count="18">
         <textField/>
         <textField/>
@@ -306,17 +308,9 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" xr16:uid="{AC2158C6-8DD2-CC45-95BF-9D9BEC4B2B61}" name="06_infectious_onbra1" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/06_infectious_onbra.txt" thousands="_x0000_" delimiter=":">
-      <textFields count="26">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
+  <connection id="10" xr16:uid="{CC6051B5-EC47-9244-A2F6-DFC847CF7A49}" name="06_infectious_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/06_infectious_not_onbra.txt" thousands=" " delimiter=":">
+      <textFields count="18">
         <textField/>
         <textField/>
         <textField/>
@@ -338,9 +332,17 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="11" xr16:uid="{D5653869-313B-0649-912D-AFDF888251AC}" name="07_SMS_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/07_SMS_not_onbra.txt" delimiter=":">
-      <textFields count="18">
+  <connection id="11" xr16:uid="{AC2158C6-8DD2-CC45-95BF-9D9BEC4B2B61}" name="06_infectious_onbra1" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/06_infectious_onbra.txt" thousands="_x0000_" delimiter=":">
+      <textFields count="26">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -362,17 +364,9 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="12" xr16:uid="{3FAA67BE-2297-B445-BDE2-D2847EE85111}" name="07_SMS_onbra1" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/07_SMS_onbra.txt" thousands="_x0000_" delimiter=":">
-      <textFields count="26">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
+  <connection id="12" xr16:uid="{D5653869-313B-0649-912D-AFDF888251AC}" name="07_SMS_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/07_SMS_not_onbra.txt" delimiter=":">
+      <textFields count="18">
         <textField/>
         <textField/>
         <textField/>
@@ -394,9 +388,17 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="13" xr16:uid="{3280E3DA-9930-5D44-8AF9-6343B3B9876C}" name="08_topology_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/08_topology_not_onbra.txt" thousands="_x0000_" delimiter=":">
-      <textFields count="18">
+  <connection id="13" xr16:uid="{3FAA67BE-2297-B445-BDE2-D2847EE85111}" name="07_SMS_onbra1" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/07_SMS_onbra.txt" thousands="_x0000_" delimiter=":">
+      <textFields count="26">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -418,8 +420,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="14" xr16:uid="{2576D0C6-56FF-C44F-8C2F-BF697E784DB8}" name="09_wiki_elections_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/09_wiki_elections_not_onbra.txt" thousands="_x0000_" delimiter=":">
+  <connection id="14" xr16:uid="{3280E3DA-9930-5D44-8AF9-6343B3B9876C}" name="08_topology_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/08_topology_not_onbra.txt" thousands="_x0000_" delimiter=":">
       <textFields count="18">
         <textField/>
         <textField/>
@@ -442,17 +444,9 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="15" xr16:uid="{AFAE3D2F-B0E6-2245-8EBD-2151221E4B12}" name="09_wiki_elections_onbra11" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/09_wiki_elections_onbra.txt" thousands="_x0000_" delimiter=":">
-      <textFields count="26">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
+  <connection id="15" xr16:uid="{2576D0C6-56FF-C44F-8C2F-BF697E784DB8}" name="09_wiki_elections_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/09_wiki_elections_not_onbra.txt" thousands="_x0000_" delimiter=":">
+      <textFields count="18">
         <textField/>
         <textField/>
         <textField/>
@@ -474,9 +468,17 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="16" xr16:uid="{8E6BAAE2-8BC9-AA4F-84AB-27A1EF1EE47A}" name="10_facebook_wall_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/10_facebook_wall_not_onbra.txt" thousands="_x0000_" delimiter=":">
-      <textFields count="18">
+  <connection id="16" xr16:uid="{AFAE3D2F-B0E6-2245-8EBD-2151221E4B12}" name="09_wiki_elections_onbra11" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/09_wiki_elections_onbra.txt" thousands="_x0000_" delimiter=":">
+      <textFields count="26">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -498,8 +500,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="17" xr16:uid="{51863DE4-76B1-DA43-9EA9-F8313722AF11}" name="11_digg_reply_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/11_digg_reply_not_onbra.txt" thousands="_x0000_" delimiter=":">
+  <connection id="17" xr16:uid="{8E6BAAE2-8BC9-AA4F-84AB-27A1EF1EE47A}" name="10_facebook_wall_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/10_facebook_wall_not_onbra.txt" thousands="_x0000_" delimiter=":">
       <textFields count="18">
         <textField/>
         <textField/>
@@ -522,8 +524,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="18" xr16:uid="{527E091F-0B51-FB44-961B-9C81979D8E9B}" name="11_digg_reply_onbra1" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/11_digg_reply_onbra.txt" thousands="_x0000_" delimiter=":">
+  <connection id="18" xr16:uid="{228A113E-18FE-564A-BB16-364A52672EBB}" name="10_facebook_wall_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/10_facebook_wall_onbra.txt" thousands="_x0000_" delimiter=":">
       <textFields count="26">
         <textField/>
         <textField/>
@@ -554,7 +556,63 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="19" xr16:uid="{C847C718-B8CE-4544-9414-400FB1205DA6}" name="12_mathoverflow_not_onbra21" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="19" xr16:uid="{51863DE4-76B1-DA43-9EA9-F8313722AF11}" name="11_digg_reply_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/11_digg_reply_not_onbra.txt" thousands="_x0000_" delimiter=":">
+      <textFields count="18">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="20" xr16:uid="{527E091F-0B51-FB44-961B-9C81979D8E9B}" name="11_digg_reply_onbra1" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/11_digg_reply_onbra.txt" thousands="_x0000_" delimiter=":">
+      <textFields count="26">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="21" xr16:uid="{C847C718-B8CE-4544-9414-400FB1205DA6}" name="12_mathoverflow_not_onbra21" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/12_mathoverflow_not_onbra.txt" thousands="_x0000_" delimiter=":">
       <textFields count="18">
         <textField/>
@@ -582,7 +640,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
   <si>
     <t>Network</t>
   </si>
@@ -750,6 +808,9 @@
   </si>
   <si>
     <t>wktau</t>
+  </si>
+  <si>
+    <t>bordeaux</t>
   </si>
 </sst>
 </file>
@@ -813,79 +874,87 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="07_SMS_not_onbra" connectionId="11" xr16:uid="{3ABAE47E-2C94-A141-99CB-25FDBEAF7C2A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="04_bordeaux_not_onbra" connectionId="9" xr16:uid="{FA2FE4D6-3B7E-7143-9596-ED826E296156}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="08_topology_not_onbra" connectionId="14" xr16:uid="{F9B28AAD-85F6-CF4C-9387-78F818EA41C7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="01_venice_not_onbra" connectionId="3" xr16:uid="{84037FAB-2A85-DD41-BA2A-5FFC56131022}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_09_wiki_elections_onbra_3" connectionId="16" xr16:uid="{82FDE27B-493D-3D4B-87B3-1418C442ED3D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="03_email_eu_onbra" connectionId="8" xr16:uid="{B954FA8F-513A-0F42-B8C0-601A4703E249}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="01_venice_onbra" connectionId="4" xr16:uid="{C8B1A7A9-6599-7C4E-A88B-D4224D9C6926}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="02_college_msg_onbra" connectionId="6" xr16:uid="{9E71A676-CDE3-514F-9D9F-D8E1F6D132D8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_11_digg_reply_onbra_3" connectionId="20" xr16:uid="{5212B2B1-13E3-C248-8185-B6CC22F101F1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="10_facebook_wall_onbra" connectionId="18" xr16:uid="{9BF26783-6509-F249-98A6-BE54F3C8611E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="07_SMS_onbra" connectionId="13" xr16:uid="{FC34ED14-BF17-014E-A08D-4091907A3CA4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="06_infectious_onbra" connectionId="11" xr16:uid="{47576FFE-E127-3E4B-A898-9923BC54421F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="10_facebook_wall_not_onbra" connectionId="17" xr16:uid="{CEC8DFA1-FE3D-D84C-86EC-707D0CFAD4F3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="00_hospital_ward_not_onbra" connectionId="2" xr16:uid="{6A109E0C-DE9A-EF4E-AE5B-5E8D7AD8CAE7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_12_mathoverflow_not_onbra_4" connectionId="21" xr16:uid="{BB3C455C-968E-CB44-8522-31B026441B37}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="07_SMS_not_onbra" connectionId="12" xr16:uid="{3ABAE47E-2C94-A141-99CB-25FDBEAF7C2A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="06_infectious_not_onbra" connectionId="10" xr16:uid="{464DFE7B-E8E0-844E-B1E6-723EBC19AC26}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="02_college_msg_not_onbra" connectionId="5" xr16:uid="{930E31CC-EC57-CD45-9F90-2DF19CECAAFC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="09_wiki_elections_not_onbra" connectionId="15" xr16:uid="{335A556A-5493-0D4F-BE56-7D42E344D12E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="00_hospital_ward_not_onbra" connectionId="1" xr16:uid="{5291992A-6D95-D042-A510-26F703B6AA8B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_11_digg_reply_onbra_3" connectionId="18" xr16:uid="{5212B2B1-13E3-C248-8185-B6CC22F101F1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="11_digg_reply_not_onbra" connectionId="19" xr16:uid="{028EAE2F-A5A1-EE41-98CA-ED564848C4F6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="06_infectious_onbra" connectionId="10" xr16:uid="{47576FFE-E127-3E4B-A898-9923BC54421F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="07_SMS_onbra" connectionId="12" xr16:uid="{FC34ED14-BF17-014E-A08D-4091907A3CA4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_09_wiki_elections_onbra_3" connectionId="15" xr16:uid="{82FDE27B-493D-3D4B-87B3-1418C442ED3D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="01_venice_onbra" connectionId="4" xr16:uid="{C8B1A7A9-6599-7C4E-A88B-D4224D9C6926}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="02_college_msg_onbra" connectionId="6" xr16:uid="{9E71A676-CDE3-514F-9D9F-D8E1F6D132D8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="03_email_eu_onbra" connectionId="8" xr16:uid="{B954FA8F-513A-0F42-B8C0-601A4703E249}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="00_hospital_ward_not_onbra" connectionId="2" xr16:uid="{6A109E0C-DE9A-EF4E-AE5B-5E8D7AD8CAE7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_12_mathoverflow_not_onbra_4" connectionId="19" xr16:uid="{BB3C455C-968E-CB44-8522-31B026441B37}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="06_infectious_not_onbra" connectionId="9" xr16:uid="{464DFE7B-E8E0-844E-B1E6-723EBC19AC26}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="03_email_eu_not_onbra" connectionId="7" xr16:uid="{A574F282-BB8A-4049-9113-0D1D5D931609}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="02_college_msg_not_onbra" connectionId="5" xr16:uid="{930E31CC-EC57-CD45-9F90-2DF19CECAAFC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="11_digg_reply_not_onbra" connectionId="17" xr16:uid="{028EAE2F-A5A1-EE41-98CA-ED564848C4F6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="01_venice_not_onbra" connectionId="3" xr16:uid="{84037FAB-2A85-DD41-BA2A-5FFC56131022}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="09_wiki_elections_not_onbra" connectionId="14" xr16:uid="{335A556A-5493-0D4F-BE56-7D42E344D12E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="08_topology_not_onbra" connectionId="13" xr16:uid="{F9B28AAD-85F6-CF4C-9387-78F818EA41C7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="10_facebook_wall_not_onbra" connectionId="16" xr16:uid="{CEC8DFA1-FE3D-D84C-86EC-707D0CFAD4F3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1185,10 +1254,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3138559-9696-A549-9DB6-01CA7B506758}">
-  <dimension ref="B2:S11"/>
+  <dimension ref="B2:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -1448,337 +1517,393 @@
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="C6" s="1">
-        <v>3389.8856999999998</v>
+        <v>43463.776700000002</v>
       </c>
       <c r="D6" s="1">
-        <v>1088.9233999999999</v>
+        <v>104.04730000000001</v>
       </c>
       <c r="E6" s="1">
-        <v>0.86</v>
+        <v>0.31</v>
       </c>
       <c r="F6" s="1">
-        <v>0.69</v>
+        <v>0.21</v>
       </c>
       <c r="G6" s="1">
-        <v>0.81</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H6" s="1">
-        <v>870.64700000000005</v>
+        <v>101.1352</v>
       </c>
       <c r="I6" s="1">
-        <v>0.79</v>
+        <v>0.44</v>
       </c>
       <c r="J6" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="L6" s="1">
+        <v>613.59990000000005</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="P6" s="1">
+        <v>3.2199999999999999E-2</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="S6" s="1">
         <v>0.61</v>
-      </c>
-      <c r="K6" s="1">
-        <v>0.76</v>
-      </c>
-      <c r="L6" s="1">
-        <v>45.956400000000002</v>
-      </c>
-      <c r="M6" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="N6" s="1">
-        <v>0.62</v>
-      </c>
-      <c r="O6" s="1">
-        <v>0.78</v>
-      </c>
-      <c r="P6" s="1">
-        <v>0.11260000000000001</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>0.66</v>
-      </c>
-      <c r="R6" s="1">
-        <v>0.48</v>
-      </c>
-      <c r="S6" s="1">
-        <v>0.65</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1">
-        <v>15198.9833</v>
+        <v>3389.8856999999998</v>
       </c>
       <c r="D7" s="1">
-        <v>3175.4782</v>
+        <v>1088.9233999999999</v>
       </c>
       <c r="E7" s="1">
-        <v>0.95</v>
+        <v>0.86</v>
       </c>
       <c r="F7" s="1">
-        <v>0.89</v>
+        <v>0.69</v>
       </c>
       <c r="G7" s="1">
-        <v>0.96</v>
+        <v>0.81</v>
       </c>
       <c r="H7" s="1">
-        <v>3757.5221000000001</v>
+        <v>870.64700000000005</v>
       </c>
       <c r="I7" s="1">
-        <v>0.93</v>
+        <v>0.79</v>
       </c>
       <c r="J7" s="1">
-        <v>0.87</v>
+        <v>0.61</v>
       </c>
       <c r="K7" s="1">
-        <v>0.95</v>
+        <v>0.76</v>
       </c>
       <c r="L7" s="1">
-        <v>635.5204</v>
+        <v>45.956400000000002</v>
       </c>
       <c r="M7" s="1">
-        <v>0.94</v>
+        <v>0.8</v>
       </c>
       <c r="N7" s="1">
-        <v>0.92</v>
+        <v>0.62</v>
       </c>
       <c r="O7" s="1">
-        <v>0.99</v>
+        <v>0.78</v>
       </c>
       <c r="P7" s="1">
-        <v>0.10879999999999999</v>
+        <v>0.11260000000000001</v>
       </c>
       <c r="Q7" s="1">
-        <v>0.86</v>
+        <v>0.66</v>
       </c>
       <c r="R7" s="1">
-        <v>0.8</v>
+        <v>0.48</v>
       </c>
       <c r="S7" s="1">
-        <v>0.94</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1">
-        <v>9486.9820999999993</v>
+        <v>15198.9833</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>3175.4782</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F8" s="1">
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="G8" s="1">
-        <v>0</v>
+        <v>0.96</v>
       </c>
       <c r="H8" s="1">
-        <v>1618.4182000000001</v>
+        <v>3757.5221000000001</v>
       </c>
       <c r="I8" s="1">
-        <v>0.78</v>
+        <v>0.93</v>
       </c>
       <c r="J8" s="1">
-        <v>0.69</v>
+        <v>0.87</v>
       </c>
       <c r="K8" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="L8" s="1">
+        <v>635.5204</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="N8" s="1">
         <v>0.92</v>
       </c>
-      <c r="L8" s="1">
-        <v>1216.579</v>
-      </c>
-      <c r="M8" s="1">
-        <v>0.76</v>
-      </c>
-      <c r="N8" s="1">
-        <v>0.66</v>
-      </c>
       <c r="O8" s="1">
-        <v>0.92</v>
+        <v>0.99</v>
       </c>
       <c r="P8" s="1">
-        <v>8.7099999999999997E-2</v>
+        <v>0.10879999999999999</v>
       </c>
       <c r="Q8" s="1">
-        <v>0.85</v>
+        <v>0.86</v>
       </c>
       <c r="R8" s="1">
-        <v>0.73</v>
+        <v>0.8</v>
       </c>
       <c r="S8" s="1">
-        <v>0.92</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1">
-        <v>606.04049999999995</v>
+        <v>9486.9820999999993</v>
       </c>
       <c r="D9" s="1">
-        <v>462.0598</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1618.4182000000001</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1216.579</v>
+      </c>
+      <c r="M9" s="1">
         <v>0.76</v>
       </c>
-      <c r="F9" s="1">
-        <v>0.71</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.94</v>
-      </c>
-      <c r="H9" s="1">
-        <v>177.9922</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0.77</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0.72</v>
-      </c>
-      <c r="K9" s="1">
-        <v>0.94</v>
-      </c>
-      <c r="L9" s="1">
-        <v>64.478399999999993</v>
-      </c>
-      <c r="M9" s="1">
-        <v>0.74</v>
-      </c>
       <c r="N9" s="1">
-        <v>0.69</v>
+        <v>0.66</v>
       </c>
       <c r="O9" s="1">
         <v>0.92</v>
       </c>
       <c r="P9" s="1">
-        <v>5.4800000000000001E-2</v>
+        <v>8.7099999999999997E-2</v>
       </c>
       <c r="Q9" s="1">
-        <v>0.76</v>
+        <v>0.85</v>
       </c>
       <c r="R9" s="1">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
       <c r="S9" s="1">
-        <v>0.94</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1">
-        <v>3079.2181</v>
+        <v>606.04049999999995</v>
       </c>
       <c r="D10" s="1">
-        <v>458.04860000000002</v>
+        <v>462.0598</v>
       </c>
       <c r="E10" s="1">
-        <v>0.96</v>
+        <v>0.76</v>
       </c>
       <c r="F10" s="1">
-        <v>0.86</v>
+        <v>0.71</v>
       </c>
       <c r="G10" s="1">
         <v>0.94</v>
       </c>
       <c r="H10" s="1">
-        <v>442.9273</v>
+        <v>177.9922</v>
       </c>
       <c r="I10" s="1">
-        <v>0.96</v>
+        <v>0.77</v>
       </c>
       <c r="J10" s="1">
-        <v>0.86</v>
+        <v>0.72</v>
       </c>
       <c r="K10" s="1">
         <v>0.94</v>
       </c>
       <c r="L10" s="1">
-        <v>500.61099999999999</v>
+        <v>64.478399999999993</v>
       </c>
       <c r="M10" s="1">
-        <v>0.97</v>
+        <v>0.74</v>
       </c>
       <c r="N10" s="1">
-        <v>0.9</v>
+        <v>0.69</v>
       </c>
       <c r="O10" s="1">
-        <v>0.96</v>
+        <v>0.92</v>
       </c>
       <c r="P10" s="1">
-        <v>5.1900000000000002E-2</v>
+        <v>5.4800000000000001E-2</v>
       </c>
       <c r="Q10" s="1">
-        <v>0.93</v>
+        <v>0.76</v>
       </c>
       <c r="R10" s="1">
-        <v>0.81</v>
+        <v>0.71</v>
       </c>
       <c r="S10" s="1">
-        <v>0.93</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1">
-        <v>1405.9414999999999</v>
+        <v>3079.2181</v>
       </c>
       <c r="D11" s="1">
-        <v>428.97640000000001</v>
+        <v>458.04860000000002</v>
       </c>
       <c r="E11" s="1">
         <v>0.96</v>
       </c>
       <c r="F11" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="H11" s="1">
+        <v>442.9273</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="L11" s="1">
+        <v>500.61099999999999</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="P11" s="1">
+        <v>5.1900000000000002E-2</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0.81</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1405.9414999999999</v>
+      </c>
+      <c r="D12" s="1">
+        <v>428.97640000000001</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="F12" s="1">
         <v>0.91</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G12" s="1">
         <v>0.96</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H12" s="1">
         <v>427.25409999999999</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I12" s="1">
         <v>0.97</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J12" s="1">
         <v>0.91</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K12" s="1">
         <v>0.96</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L12" s="1">
         <v>297.2362</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M12" s="1">
         <v>0.96</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N12" s="1">
         <v>0.95</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O12" s="1">
         <v>0.99</v>
       </c>
-      <c r="P11" s="1">
+      <c r="P12" s="1">
         <v>6.2100000000000002E-2</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="Q12" s="1">
         <v>0.94</v>
       </c>
-      <c r="R11" s="1">
+      <c r="R12" s="1">
         <v>0.89</v>
       </c>
-      <c r="S11" s="1">
+      <c r="S12" s="1">
         <v>0.96</v>
       </c>
     </row>
@@ -1792,38 +1917,24 @@
   <dimension ref="B2:AA11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="36.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="36" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="31.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="31.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="19" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="26" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -2384,6 +2495,86 @@
         <v>0.87</v>
       </c>
       <c r="AA9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3079.2181</v>
+      </c>
+      <c r="D10" s="1">
+        <v>274.37709999999998</v>
+      </c>
+      <c r="E10" s="1">
+        <v>5.3E-3</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>479.21499999999997</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1.4E-3</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
+      <c r="T10" s="1">
+        <v>971.21759999999995</v>
+      </c>
+      <c r="U10" s="1">
+        <v>3.3E-3</v>
+      </c>
+      <c r="V10" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="W10" s="1">
+        <v>0</v>
+      </c>
+      <c r="X10" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="AA10" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added BigInt ONBRA and new results and networks
</commit_message>
<xml_diff>
--- a/www/evaluation/all_but_onbra.xlsx
+++ b/www/evaluation/all_but_onbra.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/piluc/git/TSBProxy/www/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{772C727B-9A70-724D-8330-0BA284EC5894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A018ADCE-0E3B-B440-82CB-D4799374152B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="500" windowWidth="45280" windowHeight="28300" xr2:uid="{B6166BBC-CFA3-9746-8059-366614E28908}"/>
+    <workbookView xWindow="1080" yWindow="500" windowWidth="45280" windowHeight="28300" activeTab="2" xr2:uid="{B6166BBC-CFA3-9746-8059-366614E28908}"/>
   </bookViews>
   <sheets>
     <sheet name="PROXIES" sheetId="1" r:id="rId1"/>
@@ -44,6 +44,8 @@
     <definedName name="_12_mathoverflow_not_onbra_3" localSheetId="0">PROXIES!#REF!</definedName>
     <definedName name="_12_mathoverflow_not_onbra_4" localSheetId="2">'PREFIX vs PTD'!$B$3:$G$3</definedName>
     <definedName name="_12_mathoverflow_not_onbra_4" localSheetId="0">PROXIES!#REF!</definedName>
+    <definedName name="_12_mathoverflow_not_onbra_4_3" localSheetId="2">'PREFIX vs PTD'!$B$4:$G$4</definedName>
+    <definedName name="_12_mathoverflow_not_onbra_4_4" localSheetId="2">'PREFIX vs PTD'!$B$5:$G$5</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -285,7 +287,7 @@
     </textPr>
   </connection>
   <connection id="9" xr16:uid="{4221F4BE-101A-6249-9CED-0FFD2044CFDA}" name="04_bordeaux_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/04_bordeaux_not_onbra.txt" thousands="_x0000_" delimiter=":">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/04_bordeaux_not_onbra.txt" thousands="_x0000_" delimiter=":">
       <textFields count="18">
         <textField/>
         <textField/>
@@ -636,11 +638,59 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="22" xr16:uid="{AC4E96BD-BD79-2843-97F5-04FE4C1839F8}" name="12_mathoverflow_not_onbra211" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/12_mathoverflow_not_onbra.txt" thousands="_x0000_" delimiter=":">
+      <textFields count="18">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="23" xr16:uid="{E3D7C2B3-CEEC-9147-AA5D-58C9983E9A09}" name="12_mathoverflow_not_onbra212" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/12_mathoverflow_not_onbra.txt" thousands="_x0000_" delimiter=":">
+      <textFields count="18">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Network</t>
   </si>
@@ -811,13 +861,19 @@
   </si>
   <si>
     <t>bordeaux</t>
+  </si>
+  <si>
+    <t>slashdot</t>
+  </si>
+  <si>
+    <t>askubuntu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -828,6 +884,13 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -853,9 +916,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -874,75 +938,83 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="03_email_eu_not_onbra" connectionId="7" xr16:uid="{A574F282-BB8A-4049-9113-0D1D5D931609}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="11_digg_reply_not_onbra" connectionId="19" xr16:uid="{028EAE2F-A5A1-EE41-98CA-ED564848C4F6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="09_wiki_elections_not_onbra" connectionId="15" xr16:uid="{335A556A-5493-0D4F-BE56-7D42E344D12E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="02_college_msg_onbra" connectionId="6" xr16:uid="{9E71A676-CDE3-514F-9D9F-D8E1F6D132D8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="07_SMS_onbra" connectionId="13" xr16:uid="{FC34ED14-BF17-014E-A08D-4091907A3CA4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_11_digg_reply_onbra_3" connectionId="20" xr16:uid="{5212B2B1-13E3-C248-8185-B6CC22F101F1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="10_facebook_wall_onbra" connectionId="18" xr16:uid="{9BF26783-6509-F249-98A6-BE54F3C8611E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_09_wiki_elections_onbra_3" connectionId="16" xr16:uid="{82FDE27B-493D-3D4B-87B3-1418C442ED3D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="01_venice_onbra" connectionId="4" xr16:uid="{C8B1A7A9-6599-7C4E-A88B-D4224D9C6926}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="06_infectious_onbra" connectionId="11" xr16:uid="{47576FFE-E127-3E4B-A898-9923BC54421F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="03_email_eu_onbra" connectionId="8" xr16:uid="{B954FA8F-513A-0F42-B8C0-601A4703E249}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="04_bordeaux_not_onbra" connectionId="9" xr16:uid="{FA2FE4D6-3B7E-7143-9596-ED826E296156}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_12_mathoverflow_not_onbra_4_4" connectionId="23" xr16:uid="{E881FB99-ABB0-0649-BE55-098FB7183D7C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_12_mathoverflow_not_onbra_4_3" connectionId="22" xr16:uid="{90B66B99-7841-314E-A134-0C82C095EA3F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="00_hospital_ward_not_onbra" connectionId="2" xr16:uid="{6A109E0C-DE9A-EF4E-AE5B-5E8D7AD8CAE7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_12_mathoverflow_not_onbra_4" connectionId="21" xr16:uid="{BB3C455C-968E-CB44-8522-31B026441B37}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="06_infectious_not_onbra" connectionId="10" xr16:uid="{464DFE7B-E8E0-844E-B1E6-723EBC19AC26}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="10_facebook_wall_not_onbra" connectionId="17" xr16:uid="{CEC8DFA1-FE3D-D84C-86EC-707D0CFAD4F3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="08_topology_not_onbra" connectionId="14" xr16:uid="{F9B28AAD-85F6-CF4C-9387-78F818EA41C7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="01_venice_not_onbra" connectionId="3" xr16:uid="{84037FAB-2A85-DD41-BA2A-5FFC56131022}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_09_wiki_elections_onbra_3" connectionId="16" xr16:uid="{82FDE27B-493D-3D4B-87B3-1418C442ED3D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="03_email_eu_onbra" connectionId="8" xr16:uid="{B954FA8F-513A-0F42-B8C0-601A4703E249}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="01_venice_onbra" connectionId="4" xr16:uid="{C8B1A7A9-6599-7C4E-A88B-D4224D9C6926}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="02_college_msg_onbra" connectionId="6" xr16:uid="{9E71A676-CDE3-514F-9D9F-D8E1F6D132D8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_11_digg_reply_onbra_3" connectionId="20" xr16:uid="{5212B2B1-13E3-C248-8185-B6CC22F101F1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="10_facebook_wall_onbra" connectionId="18" xr16:uid="{9BF26783-6509-F249-98A6-BE54F3C8611E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="07_SMS_onbra" connectionId="13" xr16:uid="{FC34ED14-BF17-014E-A08D-4091907A3CA4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="06_infectious_onbra" connectionId="11" xr16:uid="{47576FFE-E127-3E4B-A898-9923BC54421F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="10_facebook_wall_not_onbra" connectionId="17" xr16:uid="{CEC8DFA1-FE3D-D84C-86EC-707D0CFAD4F3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="00_hospital_ward_not_onbra" connectionId="2" xr16:uid="{6A109E0C-DE9A-EF4E-AE5B-5E8D7AD8CAE7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_12_mathoverflow_not_onbra_4" connectionId="21" xr16:uid="{BB3C455C-968E-CB44-8522-31B026441B37}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="07_SMS_not_onbra" connectionId="12" xr16:uid="{3ABAE47E-2C94-A141-99CB-25FDBEAF7C2A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="06_infectious_not_onbra" connectionId="10" xr16:uid="{464DFE7B-E8E0-844E-B1E6-723EBC19AC26}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="02_college_msg_not_onbra" connectionId="5" xr16:uid="{930E31CC-EC57-CD45-9F90-2DF19CECAAFC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="09_wiki_elections_not_onbra" connectionId="15" xr16:uid="{335A556A-5493-0D4F-BE56-7D42E344D12E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -950,11 +1022,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="11_digg_reply_not_onbra" connectionId="19" xr16:uid="{028EAE2F-A5A1-EE41-98CA-ED564848C4F6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="01_venice_not_onbra" connectionId="3" xr16:uid="{84037FAB-2A85-DD41-BA2A-5FFC56131022}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="03_email_eu_not_onbra" connectionId="7" xr16:uid="{A574F282-BB8A-4049-9113-0D1D5D931609}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="07_SMS_not_onbra" connectionId="12" xr16:uid="{3ABAE47E-2C94-A141-99CB-25FDBEAF7C2A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1256,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3138559-9696-A549-9DB6-01CA7B506758}">
   <dimension ref="B2:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -2665,10 +2737,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBEDB109-7713-774E-AA4D-C88998B16425}">
-  <dimension ref="B2:G3"/>
+  <dimension ref="B2:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2721,6 +2793,46 @@
         <v>0.93</v>
       </c>
     </row>
+    <row r="4" spans="2:7" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4661.5051999999996</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.33350000000000002</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.81</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="1">
+        <v>84794.959199999998</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.81920000000000004</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Minor changes to results
</commit_message>
<xml_diff>
--- a/www/evaluation/all_but_onbra.xlsx
+++ b/www/evaluation/all_but_onbra.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/piluc/git/TSBProxy/www/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A51AA0CC-8AB3-C346-84BE-DC8995699F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{28423F81-D0C4-8F4D-9702-B1A38EC9EADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="500" windowWidth="45280" windowHeight="28300" activeTab="1" xr2:uid="{B6166BBC-CFA3-9746-8059-366614E28908}"/>
+    <workbookView xWindow="1080" yWindow="500" windowWidth="45280" windowHeight="28300" xr2:uid="{B6166BBC-CFA3-9746-8059-366614E28908}"/>
   </bookViews>
   <sheets>
     <sheet name="PROXIES" sheetId="1" r:id="rId1"/>
@@ -938,83 +938,83 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="08_topology_not_onbra" connectionId="14" xr16:uid="{F9B28AAD-85F6-CF4C-9387-78F818EA41C7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="11_digg_reply_not_onbra" connectionId="19" xr16:uid="{028EAE2F-A5A1-EE41-98CA-ED564848C4F6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="00_hospital_ward_not_onbra" connectionId="1" xr16:uid="{5291992A-6D95-D042-A510-26F703B6AA8B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_11_digg_reply_onbra_3" connectionId="20" xr16:uid="{5212B2B1-13E3-C248-8185-B6CC22F101F1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="02_college_msg_onbra" connectionId="6" xr16:uid="{9E71A676-CDE3-514F-9D9F-D8E1F6D132D8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="03_email_eu_onbra" connectionId="8" xr16:uid="{B954FA8F-513A-0F42-B8C0-601A4703E249}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="10_facebook_wall_onbra" connectionId="18" xr16:uid="{9BF26783-6509-F249-98A6-BE54F3C8611E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_09_wiki_elections_onbra_3" connectionId="16" xr16:uid="{82FDE27B-493D-3D4B-87B3-1418C442ED3D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="07_SMS_onbra" connectionId="13" xr16:uid="{FC34ED14-BF17-014E-A08D-4091907A3CA4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="06_infectious_onbra" connectionId="11" xr16:uid="{47576FFE-E127-3E4B-A898-9923BC54421F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="01_venice_onbra" connectionId="4" xr16:uid="{C8B1A7A9-6599-7C4E-A88B-D4224D9C6926}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="06_infectious_not_onbra" connectionId="10" xr16:uid="{464DFE7B-E8E0-844E-B1E6-723EBC19AC26}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_12_mathoverflow_not_onbra_4_4" connectionId="23" xr16:uid="{E881FB99-ABB0-0649-BE55-098FB7183D7C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_12_mathoverflow_not_onbra_4_3" connectionId="22" xr16:uid="{90B66B99-7841-314E-A134-0C82C095EA3F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="00_hospital_ward_not_onbra" connectionId="2" xr16:uid="{6A109E0C-DE9A-EF4E-AE5B-5E8D7AD8CAE7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_12_mathoverflow_not_onbra_4" connectionId="21" xr16:uid="{BB3C455C-968E-CB44-8522-31B026441B37}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="09_wiki_elections_not_onbra" connectionId="15" xr16:uid="{335A556A-5493-0D4F-BE56-7D42E344D12E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="01_venice_not_onbra" connectionId="3" xr16:uid="{84037FAB-2A85-DD41-BA2A-5FFC56131022}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="02_college_msg_not_onbra" connectionId="5" xr16:uid="{930E31CC-EC57-CD45-9F90-2DF19CECAAFC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="08_topology_not_onbra" connectionId="14" xr16:uid="{F9B28AAD-85F6-CF4C-9387-78F818EA41C7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="09_wiki_elections_not_onbra" connectionId="15" xr16:uid="{335A556A-5493-0D4F-BE56-7D42E344D12E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="07_SMS_onbra" connectionId="13" xr16:uid="{FC34ED14-BF17-014E-A08D-4091907A3CA4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="06_infectious_onbra" connectionId="11" xr16:uid="{47576FFE-E127-3E4B-A898-9923BC54421F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_11_digg_reply_onbra_3" connectionId="20" xr16:uid="{5212B2B1-13E3-C248-8185-B6CC22F101F1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="03_email_eu_onbra" connectionId="8" xr16:uid="{B954FA8F-513A-0F42-B8C0-601A4703E249}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="10_facebook_wall_onbra" connectionId="18" xr16:uid="{9BF26783-6509-F249-98A6-BE54F3C8611E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_09_wiki_elections_onbra_3" connectionId="16" xr16:uid="{82FDE27B-493D-3D4B-87B3-1418C442ED3D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="01_venice_onbra" connectionId="4" xr16:uid="{C8B1A7A9-6599-7C4E-A88B-D4224D9C6926}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="02_college_msg_onbra" connectionId="6" xr16:uid="{9E71A676-CDE3-514F-9D9F-D8E1F6D132D8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="03_email_eu_not_onbra" connectionId="7" xr16:uid="{A574F282-BB8A-4049-9113-0D1D5D931609}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_12_mathoverflow_not_onbra_4" connectionId="21" xr16:uid="{BB3C455C-968E-CB44-8522-31B026441B37}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_12_mathoverflow_not_onbra_4_4" connectionId="23" xr16:uid="{E881FB99-ABB0-0649-BE55-098FB7183D7C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_12_mathoverflow_not_onbra_4_3" connectionId="22" xr16:uid="{90B66B99-7841-314E-A134-0C82C095EA3F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="00_hospital_ward_not_onbra" connectionId="2" xr16:uid="{6A109E0C-DE9A-EF4E-AE5B-5E8D7AD8CAE7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="04_bordeaux_not_onbra" connectionId="9" xr16:uid="{FA2FE4D6-3B7E-7143-9596-ED826E296156}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="00_hospital_ward_not_onbra" connectionId="1" xr16:uid="{5291992A-6D95-D042-A510-26F703B6AA8B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="06_infectious_not_onbra" connectionId="10" xr16:uid="{464DFE7B-E8E0-844E-B1E6-723EBC19AC26}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="01_venice_not_onbra" connectionId="3" xr16:uid="{84037FAB-2A85-DD41-BA2A-5FFC56131022}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1022,11 +1022,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="04_bordeaux_not_onbra" connectionId="9" xr16:uid="{FA2FE4D6-3B7E-7143-9596-ED826E296156}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="10_facebook_wall_not_onbra" connectionId="17" xr16:uid="{CEC8DFA1-FE3D-D84C-86EC-707D0CFAD4F3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="11_digg_reply_not_onbra" connectionId="19" xr16:uid="{028EAE2F-A5A1-EE41-98CA-ED564848C4F6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1328,7 +1328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3138559-9696-A549-9DB6-01CA7B506758}">
   <dimension ref="B2:S12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -1988,7 +1988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAA4704-F231-804C-9F91-3ACD12F9D20A}">
   <dimension ref="B2:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB11" sqref="AB11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Only ONBRA analysis of Bordeaux missing
</commit_message>
<xml_diff>
--- a/www/evaluation/all_but_onbra.xlsx
+++ b/www/evaluation/all_but_onbra.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/piluc/git/TSBProxy/www/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28423F81-D0C4-8F4D-9702-B1A38EC9EADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{65C118DC-2383-924F-9807-A37D1EDB75EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="500" windowWidth="45280" windowHeight="28300" xr2:uid="{B6166BBC-CFA3-9746-8059-366614E28908}"/>
+    <workbookView xWindow="900" yWindow="500" windowWidth="34940" windowHeight="21900" xr2:uid="{B6166BBC-CFA3-9746-8059-366614E28908}"/>
   </bookViews>
   <sheets>
     <sheet name="PROXIES" sheetId="1" r:id="rId1"/>
@@ -28,24 +28,25 @@
     <definedName name="_03_email_eu_onbra" localSheetId="1">ONBRA!$B$5:$AA$5</definedName>
     <definedName name="_04_bordeaux_not_onbra" localSheetId="0">PROXIES!$B$6:$S$6</definedName>
     <definedName name="_06_infectious_not_onbra" localSheetId="0">PROXIES!$B$7:$S$7</definedName>
-    <definedName name="_06_infectious_onbra" localSheetId="1">ONBRA!$B$6:$AA$6</definedName>
+    <definedName name="_06_infectious_onbra" localSheetId="1">ONBRA!$B$7:$AA$7</definedName>
     <definedName name="_07_SMS_not_onbra" localSheetId="0">PROXIES!$B$8:$S$8</definedName>
-    <definedName name="_07_SMS_onbra" localSheetId="1">ONBRA!$B$7:$AA$7</definedName>
+    <definedName name="_07_SMS_onbra" localSheetId="1">ONBRA!$B$8:$AA$8</definedName>
     <definedName name="_08_topology_not_onbra" localSheetId="0">PROXIES!$B$9:$S$9</definedName>
+    <definedName name="_08_topology_onbra" localSheetId="1">ONBRA!$B$9:$AA$9</definedName>
     <definedName name="_09_wiki_elections_not_onbra" localSheetId="0">PROXIES!$B$10:$S$10</definedName>
     <definedName name="_09_wiki_elections_onbra" localSheetId="0">PROXIES!#REF!</definedName>
-    <definedName name="_09_wiki_elections_onbra_3" localSheetId="1">ONBRA!$B$9:$AA$9</definedName>
+    <definedName name="_09_wiki_elections_onbra_3" localSheetId="1">ONBRA!$B$10:$AA$10</definedName>
     <definedName name="_10_facebook_wall_not_onbra" localSheetId="0">PROXIES!$B$11:$S$11</definedName>
-    <definedName name="_10_facebook_wall_onbra" localSheetId="1">ONBRA!$B$10:$AA$10</definedName>
+    <definedName name="_10_facebook_wall_onbra" localSheetId="1">ONBRA!$B$11:$AA$11</definedName>
     <definedName name="_11_digg_reply_not_onbra" localSheetId="0">PROXIES!$B$12:$S$12</definedName>
     <definedName name="_11_digg_reply_onbra" localSheetId="1">ONBRA!#REF!</definedName>
-    <definedName name="_11_digg_reply_onbra_3" localSheetId="1">ONBRA!$B$11:$AA$11</definedName>
+    <definedName name="_11_digg_reply_onbra_3" localSheetId="1">ONBRA!$B$12:$AA$12</definedName>
     <definedName name="_12_mathoverflow_not_onbra" localSheetId="0">PROXIES!#REF!</definedName>
     <definedName name="_12_mathoverflow_not_onbra_3" localSheetId="0">PROXIES!#REF!</definedName>
     <definedName name="_12_mathoverflow_not_onbra_4" localSheetId="2">'PREFIX vs PTD'!$B$3:$G$3</definedName>
     <definedName name="_12_mathoverflow_not_onbra_4" localSheetId="0">PROXIES!#REF!</definedName>
     <definedName name="_12_mathoverflow_not_onbra_4_3" localSheetId="2">'PREFIX vs PTD'!$B$4:$G$4</definedName>
-    <definedName name="_12_mathoverflow_not_onbra_4_4" localSheetId="2">'PREFIX vs PTD'!$B$5:$G$5</definedName>
+    <definedName name="_12_mathoverflow_not_onbra_4_4" localSheetId="2">'PREFIX vs PTD'!$B$6:$G$6</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -446,9 +447,17 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="15" xr16:uid="{2576D0C6-56FF-C44F-8C2F-BF697E784DB8}" name="09_wiki_elections_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/09_wiki_elections_not_onbra.txt" thousands="_x0000_" delimiter=":">
-      <textFields count="18">
+  <connection id="15" xr16:uid="{39482123-A79D-794F-A788-882060E932AB}" name="08_topology_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/08_topology_onbra.txt" thousands="_x0000_" delimiter=":">
+      <textFields count="26">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -470,17 +479,9 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="16" xr16:uid="{AFAE3D2F-B0E6-2245-8EBD-2151221E4B12}" name="09_wiki_elections_onbra11" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/09_wiki_elections_onbra.txt" thousands="_x0000_" delimiter=":">
-      <textFields count="26">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
+  <connection id="16" xr16:uid="{2576D0C6-56FF-C44F-8C2F-BF697E784DB8}" name="09_wiki_elections_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/09_wiki_elections_not_onbra.txt" thousands="_x0000_" delimiter=":">
+      <textFields count="18">
         <textField/>
         <textField/>
         <textField/>
@@ -502,9 +503,17 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="17" xr16:uid="{8E6BAAE2-8BC9-AA4F-84AB-27A1EF1EE47A}" name="10_facebook_wall_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/10_facebook_wall_not_onbra.txt" thousands="_x0000_" delimiter=":">
-      <textFields count="18">
+  <connection id="17" xr16:uid="{AFAE3D2F-B0E6-2245-8EBD-2151221E4B12}" name="09_wiki_elections_onbra11" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/09_wiki_elections_onbra.txt" thousands="_x0000_" delimiter=":">
+      <textFields count="26">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -526,17 +535,9 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="18" xr16:uid="{228A113E-18FE-564A-BB16-364A52672EBB}" name="10_facebook_wall_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/10_facebook_wall_onbra.txt" thousands="_x0000_" delimiter=":">
-      <textFields count="26">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
+  <connection id="18" xr16:uid="{8E6BAAE2-8BC9-AA4F-84AB-27A1EF1EE47A}" name="10_facebook_wall_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/10_facebook_wall_not_onbra.txt" thousands="_x0000_" delimiter=":">
+      <textFields count="18">
         <textField/>
         <textField/>
         <textField/>
@@ -558,9 +559,17 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="19" xr16:uid="{51863DE4-76B1-DA43-9EA9-F8313722AF11}" name="11_digg_reply_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/11_digg_reply_not_onbra.txt" thousands="_x0000_" delimiter=":">
-      <textFields count="18">
+  <connection id="19" xr16:uid="{228A113E-18FE-564A-BB16-364A52672EBB}" name="10_facebook_wall_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/10_facebook_wall_onbra.txt" thousands="_x0000_" delimiter=":">
+      <textFields count="26">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -582,17 +591,9 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="20" xr16:uid="{527E091F-0B51-FB44-961B-9C81979D8E9B}" name="11_digg_reply_onbra1" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/11_digg_reply_onbra.txt" thousands="_x0000_" delimiter=":">
-      <textFields count="26">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
+  <connection id="20" xr16:uid="{51863DE4-76B1-DA43-9EA9-F8313722AF11}" name="11_digg_reply_not_onbra" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/11_digg_reply_not_onbra.txt" thousands="_x0000_" delimiter=":">
+      <textFields count="18">
         <textField/>
         <textField/>
         <textField/>
@@ -614,9 +615,17 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="21" xr16:uid="{C847C718-B8CE-4544-9414-400FB1205DA6}" name="12_mathoverflow_not_onbra21" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/12_mathoverflow_not_onbra.txt" thousands="_x0000_" delimiter=":">
-      <textFields count="18">
+  <connection id="21" xr16:uid="{527E091F-0B51-FB44-961B-9C81979D8E9B}" name="11_digg_reply_onbra1" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/11_digg_reply_onbra.txt" thousands="_x0000_" delimiter=":">
+      <textFields count="26">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -638,7 +647,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="22" xr16:uid="{AC4E96BD-BD79-2843-97F5-04FE4C1839F8}" name="12_mathoverflow_not_onbra211" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="22" xr16:uid="{C847C718-B8CE-4544-9414-400FB1205DA6}" name="12_mathoverflow_not_onbra21" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/12_mathoverflow_not_onbra.txt" thousands="_x0000_" delimiter=":">
       <textFields count="18">
         <textField/>
@@ -662,7 +671,31 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="23" xr16:uid="{E3D7C2B3-CEEC-9147-AA5D-58C9983E9A09}" name="12_mathoverflow_not_onbra212" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="23" xr16:uid="{AC4E96BD-BD79-2843-97F5-04FE4C1839F8}" name="12_mathoverflow_not_onbra211" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/12_mathoverflow_not_onbra.txt" thousands="_x0000_" delimiter=":">
+      <textFields count="18">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="24" xr16:uid="{E3D7C2B3-CEEC-9147-AA5D-58C9983E9A09}" name="12_mathoverflow_not_onbra212" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr firstRow="2" sourceFile="/Users/piluc/git/TSBProxy/www/evaluation/tmp/12_mathoverflow_not_onbra.txt" thousands="_x0000_" delimiter=":">
       <textFields count="18">
         <textField/>
@@ -690,7 +723,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
   <si>
     <t>Network</t>
   </si>
@@ -863,10 +896,13 @@
     <t>bordeaux</t>
   </si>
   <si>
-    <t>slashdot</t>
-  </si>
-  <si>
     <t>askubuntu</t>
+  </si>
+  <si>
+    <t>slashdot_reply</t>
+  </si>
+  <si>
+    <t>enron_email</t>
   </si>
 </sst>
 </file>
@@ -938,35 +974,35 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="08_topology_not_onbra" connectionId="14" xr16:uid="{F9B28AAD-85F6-CF4C-9387-78F818EA41C7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="11_digg_reply_not_onbra" connectionId="20" xr16:uid="{028EAE2F-A5A1-EE41-98CA-ED564848C4F6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="11_digg_reply_not_onbra" connectionId="19" xr16:uid="{028EAE2F-A5A1-EE41-98CA-ED564848C4F6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="10_facebook_wall_not_onbra" connectionId="18" xr16:uid="{CEC8DFA1-FE3D-D84C-86EC-707D0CFAD4F3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="00_hospital_ward_not_onbra" connectionId="1" xr16:uid="{5291992A-6D95-D042-A510-26F703B6AA8B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="01_venice_not_onbra" connectionId="3" xr16:uid="{84037FAB-2A85-DD41-BA2A-5FFC56131022}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_11_digg_reply_onbra_3" connectionId="20" xr16:uid="{5212B2B1-13E3-C248-8185-B6CC22F101F1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="08_topology_onbra" connectionId="15" xr16:uid="{D6B4C63A-2BDC-1548-965A-BF8BBB613FC9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="02_college_msg_onbra" connectionId="6" xr16:uid="{9E71A676-CDE3-514F-9D9F-D8E1F6D132D8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="03_email_eu_onbra" connectionId="8" xr16:uid="{B954FA8F-513A-0F42-B8C0-601A4703E249}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="03_email_eu_onbra" connectionId="8" xr16:uid="{B954FA8F-513A-0F42-B8C0-601A4703E249}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="01_venice_onbra" connectionId="4" xr16:uid="{C8B1A7A9-6599-7C4E-A88B-D4224D9C6926}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="10_facebook_wall_onbra" connectionId="18" xr16:uid="{9BF26783-6509-F249-98A6-BE54F3C8611E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="10_facebook_wall_onbra" connectionId="19" xr16:uid="{9BF26783-6509-F249-98A6-BE54F3C8611E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_09_wiki_elections_onbra_3" connectionId="16" xr16:uid="{82FDE27B-493D-3D4B-87B3-1418C442ED3D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_09_wiki_elections_onbra_3" connectionId="17" xr16:uid="{82FDE27B-493D-3D4B-87B3-1418C442ED3D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
@@ -974,23 +1010,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_11_digg_reply_onbra_3" connectionId="21" xr16:uid="{5212B2B1-13E3-C248-8185-B6CC22F101F1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="02_college_msg_onbra" connectionId="6" xr16:uid="{9E71A676-CDE3-514F-9D9F-D8E1F6D132D8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="02_college_msg_not_onbra" connectionId="5" xr16:uid="{930E31CC-EC57-CD45-9F90-2DF19CECAAFC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="06_infectious_onbra" connectionId="11" xr16:uid="{47576FFE-E127-3E4B-A898-9923BC54421F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="01_venice_onbra" connectionId="4" xr16:uid="{C8B1A7A9-6599-7C4E-A88B-D4224D9C6926}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="06_infectious_not_onbra" connectionId="10" xr16:uid="{464DFE7B-E8E0-844E-B1E6-723EBC19AC26}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_12_mathoverflow_not_onbra_4_4" connectionId="23" xr16:uid="{E881FB99-ABB0-0649-BE55-098FB7183D7C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_12_mathoverflow_not_onbra_4_3" connectionId="22" xr16:uid="{90B66B99-7841-314E-A134-0C82C095EA3F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_12_mathoverflow_not_onbra_4_3" connectionId="23" xr16:uid="{90B66B99-7841-314E-A134-0C82C095EA3F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
@@ -998,23 +1034,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_12_mathoverflow_not_onbra_4" connectionId="21" xr16:uid="{BB3C455C-968E-CB44-8522-31B026441B37}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_12_mathoverflow_not_onbra_4" connectionId="22" xr16:uid="{BB3C455C-968E-CB44-8522-31B026441B37}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_12_mathoverflow_not_onbra_4_4" connectionId="24" xr16:uid="{E881FB99-ABB0-0649-BE55-098FB7183D7C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="09_wiki_elections_not_onbra" connectionId="15" xr16:uid="{335A556A-5493-0D4F-BE56-7D42E344D12E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="00_hospital_ward_not_onbra" connectionId="1" xr16:uid="{5291992A-6D95-D042-A510-26F703B6AA8B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="01_venice_not_onbra" connectionId="3" xr16:uid="{84037FAB-2A85-DD41-BA2A-5FFC56131022}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="03_email_eu_not_onbra" connectionId="7" xr16:uid="{A574F282-BB8A-4049-9113-0D1D5D931609}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="02_college_msg_not_onbra" connectionId="5" xr16:uid="{930E31CC-EC57-CD45-9F90-2DF19CECAAFC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="08_topology_not_onbra" connectionId="14" xr16:uid="{F9B28AAD-85F6-CF4C-9387-78F818EA41C7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="03_email_eu_not_onbra" connectionId="7" xr16:uid="{A574F282-BB8A-4049-9113-0D1D5D931609}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="06_infectious_not_onbra" connectionId="10" xr16:uid="{464DFE7B-E8E0-844E-B1E6-723EBC19AC26}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1022,11 +1062,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="09_wiki_elections_not_onbra" connectionId="16" xr16:uid="{335A556A-5493-0D4F-BE56-7D42E344D12E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="04_bordeaux_not_onbra" connectionId="9" xr16:uid="{FA2FE4D6-3B7E-7143-9596-ED826E296156}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="10_facebook_wall_not_onbra" connectionId="17" xr16:uid="{CEC8DFA1-FE3D-D84C-86EC-707D0CFAD4F3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1328,7 +1368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3138559-9696-A549-9DB6-01CA7B506758}">
   <dimension ref="B2:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -1986,10 +2026,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAA4704-F231-804C-9F91-3ACD12F9D20A}">
-  <dimension ref="B2:AA11"/>
+  <dimension ref="B2:AA12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AB11" sqref="AB11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -2000,11 +2040,12 @@
     <col min="4" max="4" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="11" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="19" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="18" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="26" width="7.5" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="16384" width="10.83203125" style="1"/>
@@ -2332,239 +2373,244 @@
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="1">
-        <v>3389.8856999999998</v>
-      </c>
-      <c r="D6" s="1">
-        <v>23.051300000000001</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.28410000000000002</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L6" s="1">
-        <v>44.8718</v>
-      </c>
-      <c r="M6" s="1">
-        <v>0.4526</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T6" s="1">
-        <v>87.079499999999996</v>
-      </c>
-      <c r="U6" s="1">
-        <v>1.2485999999999999</v>
-      </c>
-      <c r="V6" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="W6" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="X6" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="Y6" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="Z6" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="AA6" s="1">
-        <v>0.14000000000000001</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3389.8856999999998</v>
+      </c>
+      <c r="D7" s="1">
+        <v>23.051300000000001</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.28410000000000002</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7" s="1">
+        <v>44.8718</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.4526</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T7" s="1">
+        <v>87.079499999999996</v>
+      </c>
+      <c r="U7" s="1">
+        <v>1.2485999999999999</v>
+      </c>
+      <c r="V7" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="W7" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="X7" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="1">
         <v>15198.9833</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D8" s="1">
         <v>262.1884</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E8" s="1">
         <v>12.752800000000001</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F8" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G7" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="H7" s="1">
+      <c r="G8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H8" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I7" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="J7" s="1">
+      <c r="I8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="J8" s="1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K8" s="1">
         <v>0.06</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L8" s="1">
         <v>489.81650000000002</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M8" s="1">
         <v>17.8736</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N8" s="1">
         <v>0.1</v>
       </c>
-      <c r="O7" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="P7" s="1">
+      <c r="O8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="P8" s="1">
         <v>0.09</v>
       </c>
-      <c r="Q7" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="R7" s="1">
+      <c r="Q8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="R8" s="1">
         <v>0.65</v>
       </c>
-      <c r="S7" s="1">
+      <c r="S8" s="1">
         <v>0.02</v>
       </c>
-      <c r="T7" s="1">
+      <c r="T8" s="1">
         <v>908.89459999999997</v>
       </c>
-      <c r="U7" s="1">
+      <c r="U8" s="1">
         <v>29.126899999999999</v>
       </c>
-      <c r="V7" s="1">
+      <c r="V8" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="W7" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="X7" s="1">
+      <c r="W8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="X8" s="1">
         <v>0.13</v>
       </c>
-      <c r="Y7" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="Z7" s="1">
+      <c r="Y8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="Z8" s="1">
         <v>0.72</v>
       </c>
-      <c r="AA7" s="1">
+      <c r="AA8" s="1">
         <v>0.02</v>
       </c>
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1">
-        <v>606.04049999999995</v>
+        <v>9486.9820999999993</v>
       </c>
       <c r="D9" s="1">
-        <v>29.250800000000002</v>
+        <v>544.58780000000002</v>
       </c>
       <c r="E9" s="1">
-        <v>1.5E-3</v>
+        <v>20.859000000000002</v>
       </c>
       <c r="F9" s="1">
-        <v>0.37</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="G9" s="1">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="H9" s="1">
-        <v>0.34</v>
+        <v>0.48</v>
       </c>
       <c r="I9" s="1">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="J9" s="1">
-        <v>0.8</v>
+        <v>0.88</v>
       </c>
       <c r="K9" s="1">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="L9" s="1">
-        <v>54.733499999999999</v>
+        <v>1056.0888</v>
       </c>
       <c r="M9" s="1">
-        <v>5.9999999999999995E-4</v>
+        <v>61.2134</v>
       </c>
       <c r="N9" s="1">
-        <v>0.45</v>
+        <v>0.62</v>
       </c>
       <c r="O9" s="1">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="P9" s="1">
-        <v>0.41</v>
+        <v>0.54</v>
       </c>
       <c r="Q9" s="1">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="R9" s="1">
-        <v>0.84</v>
+        <v>0.9</v>
       </c>
       <c r="S9" s="1">
         <v>0</v>
       </c>
       <c r="T9" s="1">
-        <v>105.52200000000001</v>
+        <v>2167.5207999999998</v>
       </c>
       <c r="U9" s="1">
-        <v>1.1000000000000001E-3</v>
+        <v>47.495800000000003</v>
       </c>
       <c r="V9" s="1">
-        <v>0.53</v>
+        <v>0.68</v>
       </c>
       <c r="W9" s="1">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="X9" s="1">
-        <v>0.49</v>
+        <v>0.6</v>
       </c>
       <c r="Y9" s="1">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="Z9" s="1">
-        <v>0.87</v>
+        <v>0.92</v>
       </c>
       <c r="AA9" s="1">
         <v>0</v>
@@ -2572,79 +2618,79 @@
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1">
-        <v>3079.2181</v>
+        <v>606.04049999999995</v>
       </c>
       <c r="D10" s="1">
-        <v>274.37709999999998</v>
+        <v>29.250800000000002</v>
       </c>
       <c r="E10" s="1">
-        <v>5.3E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="F10" s="1">
-        <v>0.6</v>
+        <v>0.37</v>
       </c>
       <c r="G10" s="1">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="H10" s="1">
-        <v>0.52</v>
+        <v>0.34</v>
       </c>
       <c r="I10" s="1">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="J10" s="1">
-        <v>0.88</v>
+        <v>0.8</v>
       </c>
       <c r="K10" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="L10" s="1">
-        <v>479.21499999999997</v>
+        <v>54.733499999999999</v>
       </c>
       <c r="M10" s="1">
-        <v>1.4E-3</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="N10" s="1">
-        <v>0.7</v>
+        <v>0.45</v>
       </c>
       <c r="O10" s="1">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="P10" s="1">
-        <v>0.6</v>
+        <v>0.41</v>
       </c>
       <c r="Q10" s="1">
         <v>0.01</v>
       </c>
       <c r="R10" s="1">
-        <v>0.91</v>
+        <v>0.84</v>
       </c>
       <c r="S10" s="1">
         <v>0</v>
       </c>
       <c r="T10" s="1">
-        <v>971.21759999999995</v>
+        <v>105.52200000000001</v>
       </c>
       <c r="U10" s="1">
-        <v>3.3E-3</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="V10" s="1">
-        <v>0.78</v>
+        <v>0.53</v>
       </c>
       <c r="W10" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="X10" s="1">
-        <v>0.68</v>
+        <v>0.49</v>
       </c>
       <c r="Y10" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="Z10" s="1">
-        <v>0.93</v>
+        <v>0.87</v>
       </c>
       <c r="AA10" s="1">
         <v>0</v>
@@ -2652,81 +2698,161 @@
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1">
-        <v>1405.9414999999999</v>
+        <v>3079.2181</v>
       </c>
       <c r="D11" s="1">
-        <v>110.3535</v>
+        <v>274.37709999999998</v>
       </c>
       <c r="E11" s="1">
-        <v>5.0000000000000001E-4</v>
+        <v>5.3E-3</v>
       </c>
       <c r="F11" s="1">
-        <v>0.19</v>
+        <v>0.6</v>
       </c>
       <c r="G11" s="1">
         <v>0.01</v>
       </c>
       <c r="H11" s="1">
-        <v>0.18</v>
+        <v>0.52</v>
       </c>
       <c r="I11" s="1">
         <v>0.01</v>
       </c>
       <c r="J11" s="1">
-        <v>0.74</v>
+        <v>0.88</v>
       </c>
       <c r="K11" s="1">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="L11" s="1">
-        <v>208.18350000000001</v>
+        <v>479.21499999999997</v>
       </c>
       <c r="M11" s="1">
         <v>1.4E-3</v>
       </c>
       <c r="N11" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0</v>
+      </c>
+      <c r="T11" s="1">
+        <v>971.21759999999995</v>
+      </c>
+      <c r="U11" s="1">
+        <v>3.3E-3</v>
+      </c>
+      <c r="V11" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="W11" s="1">
+        <v>0</v>
+      </c>
+      <c r="X11" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1405.9414999999999</v>
+      </c>
+      <c r="D12" s="1">
+        <v>110.3535</v>
+      </c>
+      <c r="E12" s="1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L12" s="1">
+        <v>208.18350000000001</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1.4E-3</v>
+      </c>
+      <c r="N12" s="1">
         <v>0.25</v>
       </c>
-      <c r="O11" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="P11" s="1">
+      <c r="O12" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="P12" s="1">
         <v>0.23</v>
       </c>
-      <c r="Q11" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="R11" s="1">
+      <c r="Q12" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="R12" s="1">
         <v>0.79</v>
       </c>
-      <c r="S11" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="T11" s="1">
+      <c r="S12" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="T12" s="1">
         <v>444.67099999999999</v>
       </c>
-      <c r="U11" s="1">
+      <c r="U12" s="1">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="V11" s="1">
+      <c r="V12" s="1">
         <v>0.31</v>
       </c>
-      <c r="W11" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="X11" s="1">
+      <c r="W12" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="X12" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="Y11" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="Z11" s="1">
+      <c r="Y12" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="Z12" s="1">
         <v>0.82</v>
       </c>
-      <c r="AA11" s="1">
+      <c r="AA12" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2737,10 +2863,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBEDB109-7713-774E-AA4D-C88998B16425}">
-  <dimension ref="B2:G5"/>
+  <dimension ref="B2:G6"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2795,19 +2921,19 @@
     </row>
     <row r="4" spans="2:7" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C4" s="2">
-        <v>4661.5051999999996</v>
+        <v>1100.8770999999999</v>
       </c>
       <c r="D4" s="1">
-        <v>0.33350000000000002</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="E4" s="1">
-        <v>0.81</v>
+        <v>0.88</v>
       </c>
       <c r="F4" s="1">
-        <v>0.77</v>
+        <v>0.84</v>
       </c>
       <c r="G4" s="1">
         <v>0.96</v>
@@ -2815,21 +2941,38 @@
     </row>
     <row r="5" spans="2:7" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="1">
-        <v>84794.959199999998</v>
+        <v>59</v>
+      </c>
+      <c r="C5" s="2">
+        <v>8922.3080000000009</v>
       </c>
       <c r="D5" s="1">
-        <v>0.81920000000000004</v>
+        <v>0.28260000000000002</v>
       </c>
       <c r="E5" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.49509999999999998</v>
+      </c>
+      <c r="E6" s="1">
         <v>0.74</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F6" s="1">
         <v>0.67</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G6" s="1">
         <v>0.93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added computation edges underlying graph
</commit_message>
<xml_diff>
--- a/www/evaluation/all_but_onbra.xlsx
+++ b/www/evaluation/all_but_onbra.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/piluc/git/TSBProxy/www/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5744859-3132-A749-9123-2BA525B54C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC750FC-96A5-EB47-9DCA-07383C99817E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="500" windowWidth="50120" windowHeight="28300" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="500" windowWidth="50120" windowHeight="28300" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PROXIES" sheetId="1" r:id="rId1"/>
@@ -43,13 +43,24 @@
     <definedName name="_11_digg_reply_onbra_3" localSheetId="1">ONBRA!$B$12:$AA$12</definedName>
     <definedName name="_12_mathoverflow_not_onbra" localSheetId="0">PROXIES!#REF!</definedName>
     <definedName name="_12_mathoverflow_not_onbra_3" localSheetId="0">PROXIES!#REF!</definedName>
-    <definedName name="_12_mathoverflow_not_onbra_4" localSheetId="2">'PREFIX vs PTD'!$B$3:$G$3</definedName>
+    <definedName name="_12_mathoverflow_not_onbra_4" localSheetId="2">'PREFIX vs PTD'!$B$4:$G$4</definedName>
     <definedName name="_12_mathoverflow_not_onbra_4" localSheetId="0">PROXIES!#REF!</definedName>
-    <definedName name="_12_mathoverflow_not_onbra_4_3" localSheetId="2">'PREFIX vs PTD'!$B$4:$G$4</definedName>
-    <definedName name="_12_mathoverflow_not_onbra_4_4" localSheetId="2">'PREFIX vs PTD'!$B$6:$G$6</definedName>
+    <definedName name="_12_mathoverflow_not_onbra_4_3" localSheetId="2">'PREFIX vs PTD'!$B$3:$G$3</definedName>
+    <definedName name="_12_mathoverflow_not_onbra_4_4" localSheetId="2">'PREFIX vs PTD'!$B$7:$G$7</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -602,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AMJ12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -1263,7 +1274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:AMJ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
@@ -2128,8 +2139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:G7"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2164,102 +2175,102 @@
     </row>
     <row r="3" spans="2:7" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1">
-        <v>3534.1477</v>
+        <v>1100.8770999999999</v>
       </c>
       <c r="D3" s="1">
-        <v>0.16489999999999999</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="E3" s="1">
-        <v>0.81</v>
+        <v>0.88</v>
       </c>
       <c r="F3" s="1">
-        <v>0.71</v>
+        <v>0.84</v>
       </c>
       <c r="G3" s="1">
-        <v>0.93</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="4" spans="2:7" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1">
-        <v>1100.8770999999999</v>
+        <v>3534.1477</v>
       </c>
       <c r="D4" s="1">
-        <v>0.10100000000000001</v>
+        <v>0.16489999999999999</v>
       </c>
       <c r="E4" s="1">
-        <v>0.88</v>
+        <v>0.81</v>
       </c>
       <c r="F4" s="1">
-        <v>0.84</v>
+        <v>0.71</v>
       </c>
       <c r="G4" s="1">
-        <v>0.96</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="5" spans="2:7" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C5" s="1">
-        <v>8922.3080000000009</v>
+        <v>4813.1759000000002</v>
       </c>
       <c r="D5" s="1">
-        <v>0.28260000000000002</v>
+        <v>0.28060000000000002</v>
       </c>
       <c r="E5" s="1">
-        <v>0.79</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F5" s="1">
-        <v>0.77</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G5" s="1">
-        <v>0.96</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="6" spans="2:7" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" s="1">
-        <v>37782.423000000003</v>
+        <v>8922.3081000000002</v>
       </c>
       <c r="D6" s="1">
-        <v>0.49509999999999998</v>
+        <v>0.28260000000000002</v>
       </c>
       <c r="E6" s="1">
-        <v>0.74</v>
+        <v>0.79</v>
       </c>
       <c r="F6" s="1">
-        <v>0.67</v>
+        <v>0.77</v>
       </c>
       <c r="G6" s="1">
-        <v>0.93</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="7" spans="2:7" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="1">
-        <v>4813.1759000000002</v>
+        <v>37782.423000000003</v>
       </c>
       <c r="D7" s="1">
-        <v>0.28060000000000002</v>
+        <v>0.49509999999999998</v>
       </c>
       <c r="E7" s="1">
-        <v>0.56000000000000005</v>
+        <v>0.74</v>
       </c>
       <c r="F7" s="1">
-        <v>0.55000000000000004</v>
+        <v>0.67</v>
       </c>
       <c r="G7" s="1">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>